<commit_message>
Added plot of first mode vibratoin
</commit_message>
<xml_diff>
--- a/Formal Strucutres Lab/Formal Structures Data.xlsx
+++ b/Formal Strucutres Lab/Formal Structures Data.xlsx
@@ -4,19 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="9555" windowHeight="7740" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="9555" windowHeight="7740"/>
   </bookViews>
   <sheets>
-    <sheet name="Beam" sheetId="1" r:id="rId1"/>
-    <sheet name="Wing" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="First Mode" sheetId="4" r:id="rId1"/>
+    <sheet name="Beam" sheetId="1" r:id="rId2"/>
+    <sheet name="Wing" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="E">Beam!$E$14</definedName>
+    <definedName name="rho">Beam!$E$13</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t xml:space="preserve">Length </t>
   </si>
@@ -124,6 +129,24 @@
   </si>
   <si>
     <t>(Between top of wing tip and first bend near clamp)</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>xiprime</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>y3</t>
   </si>
 </sst>
 </file>
@@ -217,22 +240,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,6 +270,322 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Theoretical</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>First</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> Mode of Vibration: Cantilever Beam</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Beam!$D$18:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.028125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0562499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0843749999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1124999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.140625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1687500000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1968750000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.2249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.2531249999999989</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.281249999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.309374999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.337499999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.365624999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.393749999999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.421874999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.449999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.478124999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.506249999999994</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.534374999999994</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.562499999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Beam!$E$18:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5874377804722995E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3543355630762654E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3658978945584999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12772831943895563</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19455125845364818</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27293770823754304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3617127585341397</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45972271662206066</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56584195012229543</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.67898044354128162</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.79809198169469009</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9221828759161883</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0503211523458966</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1816461256567621</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.3153782863493522</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4508294352564748</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5874130051728614</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.724654516581051</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.8622021222971841</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9998372045200334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="78685312"/>
+        <c:axId val="78686848"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="78685312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>X Location (in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78686848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="78686848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Y Location (in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78685312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8654143" cy="6286500"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -544,227 +890,645 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <f>20+9/16</f>
         <v>20.5625</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>1.02</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>1.875</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
         <v>0.73409999999999997</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="3">
         <f>(E3^2/(2*PI()*$B$2^2))*SQRT(($B$7*$B$5)/($B$6*$B$8))</f>
         <v>4.1566883036533238</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>5.5E-2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>4.694</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
         <v>1.0185</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="3">
         <f t="shared" ref="H4:H5" si="0">(E4^2/(2*PI()*$B$2^2))*SQRT(($B$7*$B$5)/($B$6*$B$8))</f>
         <v>26.051401115919589</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <f>(1/12)*B4^3*B3</f>
         <v>1.4141874999999999E-5</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>7.8550000000000004</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
         <v>0.99199999999999999</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
         <v>72.952015343195399</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <f>B4*B3</f>
         <v>5.6100000000000004E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <f>10*10^6</f>
         <v>10000000</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <f>25.55*10^-5</f>
         <v>2.5550000000000003E-4</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="4">
         <v>4.5</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="5">
         <f>237.2/60</f>
         <v>3.9533333333333331</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="1">
         <v>16.5</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="4">
         <f>22.5</f>
         <v>22.5</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="4">
         <f>1401/60</f>
         <v>23.35</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="1">
         <v>16.25</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="4">
         <f>67.5</f>
         <v>67.5</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="1">
         <f>3990/60</f>
         <v>66.5</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="4">
         <v>17.75</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="1">
         <v>10</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13">
+        <f>25.55*10^-5</f>
+        <v>2.5550000000000003E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <f>10*10^6</f>
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="4:7">
+      <c r="D17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7">
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <f>COSH(E$3*$D18/$B$2)-COS($D18*E$3/$B$2)-G$3*(SINH($D18*E$3/$B$2)-SIN($D18*E$3/$B$2))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <f>COSH(E$4*$D18/$B$2)-COS($D18*E$4/$B$2)-G$4*(SINH($D18*E$4/$B$2)-SIN($D18*E$4/$B$2))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <f>COSH(E$5*$D18/$B$2)-COS($D18*E$5/$B$2)-G$5*(SINH($D18*E$5/$B$2)-SIN($D18*E$5/$B$2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7">
+      <c r="D19" s="1">
+        <f>D18+($B$2/20)</f>
+        <v>1.028125</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" ref="E19:E38" si="1">COSH(E$3*$D19/$B$2)-COS($D19*E$3/$B$2)-G$3*(SINH($D19*E$3/$B$2)-SIN($D19*E$3/$B$2))</f>
+        <v>8.5874377804722995E-3</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" ref="F19:F38" si="2">COSH(E$4*$D19/$B$2)-COS($D19*E$4/$B$2)-G$4*(SINH($D19*E$4/$B$2)-SIN($D19*E$4/$B$2))</f>
+        <v>5.0695402325719618E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" ref="G19:G38" si="3">COSH(E$5*$D19/$B$2)-COS($D19*E$5/$B$2)-G$5*(SINH($D19*E$5/$B$2)-SIN($D19*E$5/$B$2))</f>
+        <v>0.13422951281811307</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7">
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:D38" si="4">D19+($B$2/20)</f>
+        <v>2.0562499999999999</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>3.3543355630762654E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.18525095578342665</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="3"/>
+        <v>0.45732873422689668</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7">
+      <c r="D21" s="1">
+        <f t="shared" si="4"/>
+        <v>3.0843749999999996</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>7.3658978945584999E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="2"/>
+        <v>0.37755393413392524</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="3"/>
+        <v>0.85358458941693449</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7">
+      <c r="D22" s="1">
+        <f t="shared" si="4"/>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>0.12772831943895563</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="2"/>
+        <v>0.60208291124702895</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2184553738105555</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7">
+      <c r="D23" s="1">
+        <f t="shared" si="4"/>
+        <v>5.140625</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>0.19455125845364818</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83447834884435867</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="3"/>
+        <v>1.467584314202119</v>
+      </c>
+    </row>
+    <row r="24" spans="4:7">
+      <c r="D24" s="1">
+        <f t="shared" si="4"/>
+        <v>6.1687500000000002</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.27293770823754304</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0522115533702401</v>
+      </c>
+      <c r="G24" s="1">
+        <f>COSH(E$5*$D24/$B$2)-COS($D24*E$5/$B$2)-G$5*(SINH($D24*E$5/$B$2)-SIN($D24*E$5/$B$2))</f>
+        <v>1.5451464301633377</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7">
+      <c r="D25" s="1">
+        <f t="shared" si="4"/>
+        <v>7.1968750000000004</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>0.3617127585341397</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2352784275018101</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4295546905140961</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7">
+      <c r="D26" s="1">
+        <f t="shared" si="4"/>
+        <v>8.2249999999999996</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>0.45972271662206066</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3668500095782914</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1352198462694965</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7">
+      <c r="D27" s="1">
+        <f t="shared" si="4"/>
+        <v>9.2531249999999989</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>0.56584195012229543</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4338194326180376</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="3"/>
+        <v>0.70985729735638969</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7">
+      <c r="D28" s="1">
+        <f t="shared" si="4"/>
+        <v>10.281249999999998</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="1"/>
+        <v>0.67898044354128162</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4271945163471802</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="3"/>
+        <v>0.22767318890568689</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7">
+      <c r="D29" s="1">
+        <f t="shared" si="4"/>
+        <v>11.309374999999998</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79809198169469009</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3422964213428354</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.22046198907161596</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7">
+      <c r="D30" s="1">
+        <f t="shared" si="4"/>
+        <v>12.337499999999997</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="1"/>
+        <v>0.9221828759161883</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1787371812816332</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.53812567540143164</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7">
+      <c r="D31" s="1">
+        <f t="shared" si="4"/>
+        <v>13.365624999999996</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0503211523458966</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="2"/>
+        <v>0.94016190519013243</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.63362336514926199</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7">
+      <c r="D32" s="1">
+        <f t="shared" si="4"/>
+        <v>14.393749999999995</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1816461256567621</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="2"/>
+        <v>0.63375434214145265</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.42718317016070273</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7">
+      <c r="D33" s="1">
+        <f t="shared" si="4"/>
+        <v>15.421874999999995</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3153782863493522</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="2"/>
+        <v>0.26951661850807085</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="3"/>
+        <v>0.14708834927819225</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7">
+      <c r="D34" s="1">
+        <f t="shared" si="4"/>
+        <v>16.449999999999996</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4508294352564748</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.14065541922495228</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1463793432802731</v>
+      </c>
+    </row>
+    <row r="35" spans="4:7">
+      <c r="D35" s="1">
+        <f t="shared" si="4"/>
+        <v>17.478124999999995</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5874130051728614</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.58407137480106996</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="3"/>
+        <v>2.6330631438921728</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7">
+      <c r="D36" s="1">
+        <f t="shared" si="4"/>
+        <v>18.506249999999994</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="1"/>
+        <v>1.724654516581051</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.0484844466467536</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="3"/>
+        <v>4.698721816215425</v>
+      </c>
+    </row>
+    <row r="37" spans="4:7">
+      <c r="D37" s="1">
+        <f t="shared" si="4"/>
+        <v>19.534374999999994</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8622021222971841</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.5234306668207722</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="3"/>
+        <v>7.4998821121238279</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7">
+      <c r="D38" s="1">
+        <f t="shared" si="4"/>
+        <v>20.562499999999993</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9998372045200334</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.0016327519389634</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="3"/>
+        <v>11.30778456277335</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7">
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -775,7 +1539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -787,84 +1551,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>7.56</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>8</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>34.4</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>35</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>50.7</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>55</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>87</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>87</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Added second and thrid modes
</commit_message>
<xml_diff>
--- a/Formal Strucutres Lab/Formal Structures Data.xlsx
+++ b/Formal Strucutres Lab/Formal Structures Data.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="9555" windowHeight="7740"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="9555" windowHeight="7740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="First Mode" sheetId="4" r:id="rId1"/>
-    <sheet name="Beam" sheetId="1" r:id="rId2"/>
-    <sheet name="Wing" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Second Mode" sheetId="5" r:id="rId2"/>
+    <sheet name="Third Mode" sheetId="6" r:id="rId3"/>
+    <sheet name="Beam" sheetId="1" r:id="rId4"/>
+    <sheet name="Wing" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="E">Beam!$E$14</definedName>
@@ -550,7 +552,585 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Theoretical</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Second</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> Mode of Vibration: Cantilever Beam</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Beam!$D$18:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.028125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0562499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0843749999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1124999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.140625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1687500000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1968750000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.2249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.2531249999999989</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.281249999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.309374999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.337499999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.365624999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.393749999999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.421874999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.449999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.478124999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.506249999999994</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.534374999999994</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.562499999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Beam!$G$18:$G$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13422951281811307</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45732873422689668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85358458941693449</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2184553738105555</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.467584314202119</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5451464301633377</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4295546905140961</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1352198462694965</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.70985729735638969</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22767318890568689</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.22046198907161596</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.53812567540143164</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.63362336514926199</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.42718317016070273</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.14708834927819225</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1463793432802731</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.6330631438921728</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.698721816215425</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.4998821121238279</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11.30778456277335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="123406976"/>
+        <c:axId val="130884352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="123406976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>X Location (in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="130884352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="130884352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Y Location (in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="123406976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Theoretical</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Third</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> Mode of Vibration: Cantilever Beam</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Beam!$D$18:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.028125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0562499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0843749999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1124999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.140625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1687500000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1968750000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.2249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.2531249999999989</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.281249999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.309374999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.337499999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.365624999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.393749999999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.421874999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.449999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.478124999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.506249999999994</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.534374999999994</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.562499999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Beam!$G$18:$G$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13422951281811307</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45732873422689668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85358458941693449</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2184553738105555</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.467584314202119</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5451464301633377</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4295546905140961</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1352198462694965</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.70985729735638969</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22767318890568689</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.22046198907161596</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.53812567540143164</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.63362336514926199</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.42718317016070273</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.14708834927819225</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1463793432802731</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.6330631438921728</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.698721816215425</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.4998821121238279</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11.30778456277335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="78612736"/>
+        <c:axId val="78693888"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="78612736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>X Location (in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78693888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="78693888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Y Location (in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78612736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -566,6 +1146,60 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
     <xdr:ext cx="8654143" cy="6286500"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8665104" cy="6283854"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8665104" cy="6283854"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -875,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:E38"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G18" activeCellId="1" sqref="D18:D38 G18:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1511,7 +2145,7 @@
         <v>1.9998372045200334</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="2"/>
+        <f>COSH(E$4*$D38/$B$2)-COS($D38*E$4/$B$2)-G$4*(SINH($D38*E$4/$B$2)-SIN($D38*E$4/$B$2))</f>
         <v>-2.0016327519389634</v>
       </c>
       <c r="G38" s="1">

</xml_diff>